<commit_message>
restarted on generic compositions - need to correlate access properly with super classes
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_All_Short_Solutions.xlsx
+++ b/data/TR/results/PVRP_All_Short_Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="13">
   <si>
     <t>Filename</t>
   </si>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B7" t="n">
         <v>-1.0</v>
@@ -2634,93 +2634,87 @@
         <v>0.0</v>
       </c>
       <c r="D7" t="n">
-        <v>540.0</v>
+        <v>469.0</v>
       </c>
       <c r="E7" t="n">
         <v>-1.0</v>
       </c>
       <c r="F7" t="n">
-        <v>13.0</v>
+        <v>4.0</v>
       </c>
       <c r="G7" t="n">
-        <v>25.0</v>
+        <v>14.0</v>
       </c>
       <c r="H7" t="n">
-        <v>14.0</v>
+        <v>6.0</v>
       </c>
       <c r="I7" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="J7" t="n">
-        <v>43.0</v>
+        <v>51.0</v>
       </c>
       <c r="K7" t="n">
-        <v>23.0</v>
+        <v>32.0</v>
       </c>
       <c r="L7" t="n">
-        <v>7.0</v>
+        <v>26.0</v>
       </c>
       <c r="M7" t="n">
-        <v>26.0</v>
+        <v>22.0</v>
       </c>
       <c r="N7" t="n">
-        <v>48.0</v>
+        <v>28.0</v>
       </c>
       <c r="O7" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="P7" t="n">
-        <v>22.0</v>
+        <v>36.0</v>
       </c>
       <c r="Q7" t="n">
-        <v>31.0</v>
+        <v>35.0</v>
       </c>
       <c r="R7" t="n">
-        <v>28.0</v>
+        <v>20.0</v>
       </c>
       <c r="S7" t="n">
-        <v>36.0</v>
+        <v>2.0</v>
       </c>
       <c r="T7" t="n">
-        <v>20.0</v>
+        <v>50.0</v>
       </c>
       <c r="U7" t="n">
-        <v>32.0</v>
+        <v>9.0</v>
       </c>
       <c r="V7" t="n">
-        <v>46.0</v>
+        <v>10.0</v>
       </c>
       <c r="W7" t="n">
-        <v>51.0</v>
+        <v>5.0</v>
       </c>
       <c r="X7" t="n">
-        <v>47.0</v>
+        <v>12.0</v>
       </c>
       <c r="Y7" t="n">
-        <v>12.0</v>
+        <v>17.0</v>
       </c>
       <c r="Z7" t="n">
-        <v>39.0</v>
+        <v>37.0</v>
       </c>
       <c r="AA7" t="n">
-        <v>33.0</v>
+        <v>15.0</v>
       </c>
       <c r="AB7" t="n">
-        <v>44.0</v>
+        <v>42.0</v>
       </c>
       <c r="AC7" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="AE7" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B8" t="n">
         <v>-1.0</v>
@@ -2729,96 +2723,102 @@
         <v>1.0</v>
       </c>
       <c r="D8" t="n">
-        <v>397.0</v>
+        <v>468.0</v>
       </c>
       <c r="E8" t="n">
         <v>-1.0</v>
       </c>
       <c r="F8" t="n">
-        <v>45.0</v>
+        <v>41.0</v>
       </c>
       <c r="G8" t="n">
-        <v>15.0</v>
+        <v>13.0</v>
       </c>
       <c r="H8" t="n">
-        <v>5.0</v>
+        <v>47.0</v>
       </c>
       <c r="I8" t="n">
-        <v>49.0</v>
+        <v>18.0</v>
       </c>
       <c r="J8" t="n">
-        <v>10.0</v>
+        <v>25.0</v>
       </c>
       <c r="K8" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="V8" t="n">
         <v>30.0</v>
       </c>
-      <c r="L8" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="Q8" t="n">
+      <c r="W8" t="n">
         <v>16.0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="T8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="U8" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="V8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="W8" t="n">
-        <v>27.0</v>
       </c>
       <c r="X8" t="n">
         <v>11.0</v>
       </c>
       <c r="Y8" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="Z8" t="n">
         <v>38.0</v>
       </c>
-      <c r="Z8" t="n">
-        <v>37.0</v>
-      </c>
       <c r="AA8" t="n">
-        <v>17.0</v>
+        <v>49.0</v>
       </c>
       <c r="AB8" t="n">
-        <v>18.0</v>
+        <v>39.0</v>
       </c>
       <c r="AC8" t="n">
-        <v>41.0</v>
+        <v>33.0</v>
       </c>
       <c r="AD8" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="AF8" t="n">
         <v>19.0</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AG8" t="n">
         <v>40.0</v>
       </c>
-      <c r="AF8" t="n">
+      <c r="AH8" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B9" t="n">
         <v>-1.0</v>
@@ -2827,93 +2827,87 @@
         <v>2.0</v>
       </c>
       <c r="D9" t="n">
-        <v>540.0</v>
+        <v>469.0</v>
       </c>
       <c r="E9" t="n">
         <v>-1.0</v>
       </c>
       <c r="F9" t="n">
-        <v>13.0</v>
+        <v>4.0</v>
       </c>
       <c r="G9" t="n">
-        <v>25.0</v>
+        <v>14.0</v>
       </c>
       <c r="H9" t="n">
-        <v>14.0</v>
+        <v>6.0</v>
       </c>
       <c r="I9" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="J9" t="n">
-        <v>43.0</v>
+        <v>51.0</v>
       </c>
       <c r="K9" t="n">
-        <v>23.0</v>
+        <v>32.0</v>
       </c>
       <c r="L9" t="n">
-        <v>7.0</v>
+        <v>26.0</v>
       </c>
       <c r="M9" t="n">
-        <v>26.0</v>
+        <v>22.0</v>
       </c>
       <c r="N9" t="n">
-        <v>48.0</v>
+        <v>28.0</v>
       </c>
       <c r="O9" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="P9" t="n">
-        <v>22.0</v>
+        <v>36.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>31.0</v>
+        <v>35.0</v>
       </c>
       <c r="R9" t="n">
-        <v>28.0</v>
+        <v>20.0</v>
       </c>
       <c r="S9" t="n">
-        <v>36.0</v>
+        <v>2.0</v>
       </c>
       <c r="T9" t="n">
-        <v>20.0</v>
+        <v>50.0</v>
       </c>
       <c r="U9" t="n">
-        <v>32.0</v>
+        <v>9.0</v>
       </c>
       <c r="V9" t="n">
-        <v>46.0</v>
+        <v>10.0</v>
       </c>
       <c r="W9" t="n">
-        <v>51.0</v>
+        <v>5.0</v>
       </c>
       <c r="X9" t="n">
-        <v>47.0</v>
+        <v>12.0</v>
       </c>
       <c r="Y9" t="n">
-        <v>12.0</v>
+        <v>17.0</v>
       </c>
       <c r="Z9" t="n">
-        <v>39.0</v>
+        <v>37.0</v>
       </c>
       <c r="AA9" t="n">
-        <v>33.0</v>
+        <v>15.0</v>
       </c>
       <c r="AB9" t="n">
-        <v>44.0</v>
+        <v>42.0</v>
       </c>
       <c r="AC9" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="AE9" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B10" t="n">
         <v>-1.0</v>
@@ -2922,96 +2916,102 @@
         <v>3.0</v>
       </c>
       <c r="D10" t="n">
-        <v>397.0</v>
+        <v>468.0</v>
       </c>
       <c r="E10" t="n">
         <v>-1.0</v>
       </c>
       <c r="F10" t="n">
-        <v>45.0</v>
+        <v>41.0</v>
       </c>
       <c r="G10" t="n">
-        <v>15.0</v>
+        <v>13.0</v>
       </c>
       <c r="H10" t="n">
-        <v>5.0</v>
+        <v>47.0</v>
       </c>
       <c r="I10" t="n">
-        <v>49.0</v>
+        <v>18.0</v>
       </c>
       <c r="J10" t="n">
-        <v>10.0</v>
+        <v>25.0</v>
       </c>
       <c r="K10" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="V10" t="n">
         <v>30.0</v>
       </c>
-      <c r="L10" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="Q10" t="n">
+      <c r="W10" t="n">
         <v>16.0</v>
-      </c>
-      <c r="R10" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="S10" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="T10" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="U10" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="V10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="W10" t="n">
-        <v>27.0</v>
       </c>
       <c r="X10" t="n">
         <v>11.0</v>
       </c>
       <c r="Y10" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="Z10" t="n">
         <v>38.0</v>
       </c>
-      <c r="Z10" t="n">
-        <v>37.0</v>
-      </c>
       <c r="AA10" t="n">
-        <v>17.0</v>
+        <v>49.0</v>
       </c>
       <c r="AB10" t="n">
-        <v>18.0</v>
+        <v>39.0</v>
       </c>
       <c r="AC10" t="n">
-        <v>41.0</v>
+        <v>33.0</v>
       </c>
       <c r="AD10" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="AF10" t="n">
         <v>19.0</v>
       </c>
-      <c r="AE10" t="n">
+      <c r="AG10" t="n">
         <v>40.0</v>
       </c>
-      <c r="AF10" t="n">
+      <c r="AH10" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B11" t="n">
         <v>-1.0</v>
@@ -3020,93 +3020,87 @@
         <v>4.0</v>
       </c>
       <c r="D11" t="n">
-        <v>540.0</v>
+        <v>469.0</v>
       </c>
       <c r="E11" t="n">
         <v>-1.0</v>
       </c>
       <c r="F11" t="n">
-        <v>13.0</v>
+        <v>4.0</v>
       </c>
       <c r="G11" t="n">
-        <v>25.0</v>
+        <v>14.0</v>
       </c>
       <c r="H11" t="n">
-        <v>14.0</v>
+        <v>6.0</v>
       </c>
       <c r="I11" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="J11" t="n">
-        <v>43.0</v>
+        <v>51.0</v>
       </c>
       <c r="K11" t="n">
-        <v>23.0</v>
+        <v>32.0</v>
       </c>
       <c r="L11" t="n">
-        <v>7.0</v>
+        <v>26.0</v>
       </c>
       <c r="M11" t="n">
-        <v>26.0</v>
+        <v>22.0</v>
       </c>
       <c r="N11" t="n">
-        <v>48.0</v>
+        <v>28.0</v>
       </c>
       <c r="O11" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="P11" t="n">
-        <v>22.0</v>
+        <v>36.0</v>
       </c>
       <c r="Q11" t="n">
-        <v>31.0</v>
+        <v>35.0</v>
       </c>
       <c r="R11" t="n">
-        <v>28.0</v>
+        <v>20.0</v>
       </c>
       <c r="S11" t="n">
-        <v>36.0</v>
+        <v>2.0</v>
       </c>
       <c r="T11" t="n">
-        <v>20.0</v>
+        <v>50.0</v>
       </c>
       <c r="U11" t="n">
-        <v>32.0</v>
+        <v>9.0</v>
       </c>
       <c r="V11" t="n">
-        <v>46.0</v>
+        <v>10.0</v>
       </c>
       <c r="W11" t="n">
-        <v>51.0</v>
+        <v>5.0</v>
       </c>
       <c r="X11" t="n">
-        <v>47.0</v>
+        <v>12.0</v>
       </c>
       <c r="Y11" t="n">
-        <v>12.0</v>
+        <v>17.0</v>
       </c>
       <c r="Z11" t="n">
-        <v>39.0</v>
+        <v>37.0</v>
       </c>
       <c r="AA11" t="n">
-        <v>33.0</v>
+        <v>15.0</v>
       </c>
       <c r="AB11" t="n">
-        <v>44.0</v>
+        <v>42.0</v>
       </c>
       <c r="AC11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="AE11" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B12" t="n">
         <v>-1.0</v>
@@ -3115,90 +3109,96 @@
         <v>5.0</v>
       </c>
       <c r="D12" t="n">
-        <v>397.0</v>
+        <v>468.0</v>
       </c>
       <c r="E12" t="n">
         <v>-1.0</v>
       </c>
       <c r="F12" t="n">
-        <v>45.0</v>
+        <v>41.0</v>
       </c>
       <c r="G12" t="n">
-        <v>15.0</v>
+        <v>13.0</v>
       </c>
       <c r="H12" t="n">
-        <v>5.0</v>
+        <v>47.0</v>
       </c>
       <c r="I12" t="n">
-        <v>49.0</v>
+        <v>18.0</v>
       </c>
       <c r="J12" t="n">
-        <v>10.0</v>
+        <v>25.0</v>
       </c>
       <c r="K12" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="V12" t="n">
         <v>30.0</v>
       </c>
-      <c r="L12" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="Q12" t="n">
+      <c r="W12" t="n">
         <v>16.0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="T12" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="W12" t="n">
-        <v>27.0</v>
       </c>
       <c r="X12" t="n">
         <v>11.0</v>
       </c>
       <c r="Y12" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="Z12" t="n">
         <v>38.0</v>
       </c>
-      <c r="Z12" t="n">
-        <v>37.0</v>
-      </c>
       <c r="AA12" t="n">
-        <v>17.0</v>
+        <v>49.0</v>
       </c>
       <c r="AB12" t="n">
-        <v>18.0</v>
+        <v>39.0</v>
       </c>
       <c r="AC12" t="n">
-        <v>41.0</v>
+        <v>33.0</v>
       </c>
       <c r="AD12" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="AF12" t="n">
         <v>19.0</v>
       </c>
-      <c r="AE12" t="n">
+      <c r="AG12" t="n">
         <v>40.0</v>
       </c>
-      <c r="AF12" t="n">
+      <c r="AH12" t="n">
         <v>-1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
everything back up and running properly now -- need local op
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_All_Short_Solutions.xlsx
+++ b/data/TR/results/PVRP_All_Short_Solutions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Filename</t>
   </si>
@@ -149,12 +149,24 @@
         <v>0.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>125.0</v>
       </c>
       <c r="E7" t="n">
         <v>-1.0</v>
       </c>
       <c r="F7" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="J7" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -169,12 +181,33 @@
         <v>1.0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>141.0</v>
       </c>
       <c r="E8" t="n">
         <v>-1.0</v>
       </c>
       <c r="F8" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="M8" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -189,12 +222,36 @@
         <v>2.0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>150.0</v>
       </c>
       <c r="E9" t="n">
         <v>-1.0</v>
       </c>
       <c r="F9" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="N9" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -209,12 +266,39 @@
         <v>3.0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>144.0</v>
       </c>
       <c r="E10" t="n">
         <v>-1.0</v>
       </c>
       <c r="F10" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="O10" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -229,12 +313,33 @@
         <v>4.0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>81.0</v>
       </c>
       <c r="E11" t="n">
         <v>-1.0</v>
       </c>
       <c r="F11" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="M11" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -249,12 +354,30 @@
         <v>5.0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>92.0</v>
       </c>
       <c r="E12" t="n">
         <v>-1.0</v>
       </c>
       <c r="F12" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="L12" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -269,12 +392,30 @@
         <v>6.0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>151.0</v>
       </c>
       <c r="E13" t="n">
         <v>-1.0</v>
       </c>
       <c r="F13" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="L13" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -289,12 +430,36 @@
         <v>7.0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>153.0</v>
       </c>
       <c r="E14" t="n">
         <v>-1.0</v>
       </c>
       <c r="F14" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="N14" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -309,12 +474,30 @@
         <v>8.0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0</v>
+        <v>153.0</v>
       </c>
       <c r="E15" t="n">
         <v>-1.0</v>
       </c>
       <c r="F15" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="L15" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -329,12 +512,33 @@
         <v>9.0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>146.0</v>
       </c>
       <c r="E16" t="n">
         <v>-1.0</v>
       </c>
       <c r="F16" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="M16" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -349,12 +553,33 @@
         <v>10.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>124.0</v>
       </c>
       <c r="E17" t="n">
         <v>-1.0</v>
       </c>
       <c r="F17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="M17" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -369,12 +594,42 @@
         <v>11.0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0</v>
+        <v>157.0</v>
       </c>
       <c r="E18" t="n">
         <v>-1.0</v>
       </c>
       <c r="F18" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="P18" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -389,12 +644,33 @@
         <v>12.0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
+        <v>151.0</v>
       </c>
       <c r="E19" t="n">
         <v>-1.0</v>
       </c>
       <c r="F19" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="M19" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -409,12 +685,36 @@
         <v>13.0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0</v>
+        <v>159.0</v>
       </c>
       <c r="E20" t="n">
         <v>-1.0</v>
       </c>
       <c r="F20" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="N20" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -429,12 +729,24 @@
         <v>14.0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0</v>
+        <v>125.0</v>
       </c>
       <c r="E21" t="n">
         <v>-1.0</v>
       </c>
       <c r="F21" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="J21" t="n">
         <v>-1.0</v>
       </c>
     </row>

</xml_diff>